<commit_message>
Modify HIV prevalence distribution among male partners
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Dropbox/UW Epi Program/RB/sources-eff-dilution-ring/ring-eff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Documents/code/aspire/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -41,17 +41,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Baeten, 2016</t>
-  </si>
-  <si>
-    <t>Baeten, 2016 states that approximately 85% of women were retained in the study. In our model, retention at each time step is a random binomial draw. We therefore need a probability of loss-to-follow-up per time step, assuming a constant rate of loss to follow-up.  We estimate the parameter here as follows:
-0.15 = 1 - exp(-37*lambda) --&gt; lambda = 0.004392403
-probability of loss to follow-up per time step: p = 1 - exp(-0.004392403) --&gt; 0.004382771</t>
-  </si>
-  <si>
-    <t>loss_to_fup_prob</t>
-  </si>
-  <si>
     <t>lambda</t>
   </si>
   <si>
@@ -65,13 +54,25 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>cond_rr</t>
+  </si>
+  <si>
+    <t>Relative increase in probability of having an HIV-positive male partner among those who report using condoms in previous week at baseline, relative to those who report not using condoms in previous 7 days at baseline.</t>
+  </si>
+  <si>
+    <t>pre_adh_int_rr_bl</t>
+  </si>
+  <si>
+    <t>pre_adh_int_rr_fu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,12 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,6 +130,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -400,21 +401,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="112.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,52 +429,65 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1.8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>4.3827709999999997E-3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
+      <c r="B8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify HIV risk by age; bug fix
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3.0000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -445,7 +445,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -453,7 +453,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
Calculate likelihood using placebo arm only; fix merge statements in hiv_transmission fx
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -405,7 +405,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.15</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -480,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.9</v>
+        <v>3.0550000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -488,7 +488,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functions/code for secondary analysis
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Documents/code/aspire/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2226855B-C035-B243-8A2A-E899BE1A97B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA27E7F-E37D-4E4B-83D8-F1602309590F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="195">
   <si>
     <t>name</t>
   </si>
@@ -43,15 +42,9 @@
     <t>lambda</t>
   </si>
   <si>
-    <t>Boily</t>
-  </si>
-  <si>
     <t>cond_rr</t>
   </si>
   <si>
-    <t>Relative increase in probability of having an HIV-positive male partner among those who report using condoms in previous week at baseline, relative to those who report not using condoms in previous 7 days at baseline.</t>
-  </si>
-  <si>
     <t>Predictive model from Elizabeth Brown</t>
   </si>
   <si>
@@ -550,12 +543,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>Carrying capacity term used in inverse logistic-like function to assign relative probability of having an HIV-positive male partner</t>
-  </si>
-  <si>
-    <t>Scale parameter term used in inverse logistic-like function to assign relative probability of having an HIV-positive male partner</t>
-  </si>
-  <si>
     <t>Calibrated in ABC model-fitting procedure with priors in uniform[0,1]</t>
   </si>
   <si>
@@ -574,9 +561,6 @@
     <t>pm_adhfu_Spilhaus</t>
   </si>
   <si>
-    <t>Calibrated in ABC model-fitting procedure with priors in ????</t>
-  </si>
-  <si>
     <t>rr_ai</t>
   </si>
   <si>
@@ -586,9 +570,6 @@
     <t>rr_age</t>
   </si>
   <si>
-    <t>rr_ring</t>
-  </si>
-  <si>
     <t>rr_condom</t>
   </si>
   <si>
@@ -599,6 +580,36 @@
   </si>
   <si>
     <t>Hughes, 2012</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with priors in uniform[1,3]</t>
+  </si>
+  <si>
+    <t>Relative increase in probability of having an HIV-positive male partner among those who report using condoms in previous week at baseline, relative to those who report not using condoms in previous 7 days at baseline. In ABC process, we use a uniform prior in [1,3] because relative risk associated with condom use should not be lower than 1, and cannot be higher than 3.34 in order to constrain prevalence probability draws to &lt;= 1.</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with priors in uniform[5,16]</t>
+  </si>
+  <si>
+    <t>Carrying capacity term used in inverse logistic-like function to assign relative probability of having an HIV-positive male partner given age</t>
+  </si>
+  <si>
+    <t>Scale parameter term used in inverse logistic-like function to assign relative probability of having an HIV-positive male partner given age</t>
+  </si>
+  <si>
+    <t>Boily, 2009</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with beta distribution with parameters alpha = 5 and beta = 1664, corresponding to point estimate and confidence interval reported for male-female-transmission in LMIC in Boily meta-analysis.</t>
+  </si>
+  <si>
+    <t>Brown, unpublished</t>
+  </si>
+  <si>
+    <t>rr_ring_full_adh</t>
+  </si>
+  <si>
+    <t>rr_ring_partial_adh</t>
   </si>
 </sst>
 </file>
@@ -608,7 +619,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -966,14 +977,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -981,7 +992,7 @@
     <col min="4" max="4" width="112.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -995,1420 +1006,1428 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>2.5000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>1.8</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3">
         <v>0.95</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5" s="3">
         <v>0.45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B6" s="3">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B7" s="3">
         <v>2.89</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B8" s="3">
         <v>0.96</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B9" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B10" s="3">
-        <v>0.22</v>
+        <v>0.5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B11" s="3">
-        <v>2.5</v>
+        <v>0.22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B12" s="3">
-        <v>3.63</v>
+        <v>2.5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.63</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="2">
         <v>1.26217</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="2">
         <v>6.4359999999999999E-3</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2.4802000000000001E-2</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
-        <v>-0.50241100000000005</v>
+        <v>2.4802000000000001E-2</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
-        <v>-0.51592700000000002</v>
+        <v>-0.50241100000000005</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2">
-        <v>-0.121917</v>
+        <v>-0.51592700000000002</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2">
-        <v>0.11065899999999999</v>
+        <v>-0.121917</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
-        <v>-9.4164999999999999E-2</v>
+        <v>0.11065899999999999</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2">
-        <v>-0.28917900000000002</v>
+        <v>-9.4164999999999999E-2</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2">
-        <v>-5.6791000000000001E-2</v>
+        <v>-0.28917900000000002</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2">
-        <v>-0.32421</v>
+        <v>-5.6791000000000001E-2</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B24" s="2">
-        <v>0.14365600000000001</v>
+        <v>-0.32421</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="B25" s="2">
-        <v>0.90519000000000005</v>
+        <v>0.14365600000000001</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2">
-        <v>0.26147399999999998</v>
+        <v>0.90519000000000005</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2">
-        <v>0.41216000000000003</v>
+        <v>0.26147399999999998</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2">
-        <v>-0.26832899999999998</v>
+        <v>0.41216000000000003</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2">
-        <v>0.93457599999999996</v>
+        <v>-0.26832899999999998</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>179</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2">
-        <v>-1.047471</v>
+        <v>0.93457599999999996</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="B31" s="2">
-        <v>-0.17377999999999999</v>
+        <v>-1.047471</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B32" s="2">
-        <v>-0.77863599999999999</v>
+        <v>-0.17377999999999999</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2">
-        <v>-0.83789400000000003</v>
+        <v>-0.77863599999999999</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B34" s="2">
-        <v>-0.20571900000000001</v>
+        <v>-0.83789400000000003</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2">
-        <v>-3.8223E-2</v>
+        <v>-0.20571900000000001</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2">
-        <v>0.19087599999999999</v>
+        <v>-3.8223E-2</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B37" s="2">
-        <v>-5.3702E-2</v>
+        <v>0.19087599999999999</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2">
-        <v>0.32832800000000001</v>
+        <v>-5.3702E-2</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B39" s="2">
-        <v>0.57400700000000004</v>
+        <v>0.32832800000000001</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="4">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.57400700000000004</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="4">
         <v>-17.1313</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="4">
-        <v>14.75226</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B42" s="4">
-        <v>4.0779999999999997E-2</v>
+        <f>14.75226+0.70075</f>
+        <v>15.453009999999999</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B43" s="4">
-        <v>8.8822700000000001</v>
+        <v>4.0779999999999997E-2</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B44" s="4">
-        <v>2.9960000000000001E-2</v>
+        <v>8.8822700000000001</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>165</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B45" s="4">
-        <v>0.92173000000000005</v>
+        <v>2.9960000000000001E-2</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B46" s="4">
-        <v>0.6411</v>
+        <v>0.92173000000000005</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B47" s="4">
-        <v>2.53809</v>
+        <v>0.6411</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B48" s="4">
-        <v>0.42286000000000001</v>
+        <v>2.53809</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B49" s="4">
-        <v>2.3041399999999999</v>
+        <v>0.42286000000000001</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B50" s="4">
-        <v>-0.26913999999999999</v>
+        <v>2.3041399999999999</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B51" s="4">
-        <v>-0.19550000000000001</v>
+        <v>-0.26913999999999999</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B52" s="4">
-        <v>0.18842999999999999</v>
+        <v>-0.19550000000000001</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>165</v>
+        <v>68</v>
       </c>
       <c r="B53" s="4">
-        <v>-0.97519</v>
+        <v>0.18842999999999999</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B54" s="4">
-        <v>0.83792999999999995</v>
+        <v>-0.97519</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="B55" s="4">
-        <v>-1.2729200000000001</v>
+        <v>0.83792999999999995</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B56" s="4">
-        <v>2.4960499999999999</v>
+        <v>-1.2729200000000001</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B57" s="4">
-        <v>2.62182</v>
+        <v>2.4960499999999999</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B58" s="4">
-        <v>1.36452</v>
+        <v>2.62182</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B59" s="4">
-        <v>0.19872000000000001</v>
+        <v>1.36452</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>180</v>
+        <v>73</v>
       </c>
       <c r="B60" s="4">
-        <v>1.2533799999999999</v>
+        <v>0.19872000000000001</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="B61" s="4">
-        <v>-1.2487600000000001</v>
+        <v>1.2533799999999999</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B62" s="4">
-        <v>0.91396999999999995</v>
+        <v>-1.2487600000000001</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B63" s="4">
-        <v>-0.65583000000000002</v>
+        <v>0.91396999999999995</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B64" s="4">
-        <v>-0.61004000000000003</v>
+        <v>-0.65583000000000002</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B65" s="4">
-        <v>-0.20158999999999999</v>
+        <v>-0.61004000000000003</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B66" s="4">
-        <v>0.53534999999999999</v>
+        <v>-0.20158999999999999</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B67" s="4">
-        <v>1.72922</v>
+        <v>0.53534999999999999</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="B68" s="4">
-        <v>-0.61790999999999996</v>
+        <v>1.72922</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>83</v>
+        <v>177</v>
       </c>
       <c r="B69" s="4">
-        <v>-1.86713</v>
+        <v>-0.61790999999999996</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="4">
+        <v>-1.86713</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="1">
         <v>-1.4727514500000001</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="1">
+      <c r="C71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="1">
         <v>-2.2884722900000001</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.62259118000000002</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B73" s="1">
-        <v>0.75163418000000004</v>
+        <v>0.62259118000000002</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B74" s="1">
-        <v>-0.28502549999999999</v>
+        <v>0.75163418000000004</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B75" s="1">
-        <v>-0.32447941000000002</v>
+        <v>-0.28502549999999999</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B76" s="1">
-        <v>3.1312599999999999E-3</v>
+        <v>-0.32447941000000002</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B77" s="1">
-        <v>1.5448442099999999</v>
+        <v>3.1312599999999999E-3</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B78" s="3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1.5448442099999999</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="3">
         <v>-1.7325664999999999</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" s="3">
+      <c r="C79" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80" s="3">
         <v>-8.9997569999999999E-2</v>
-      </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B80" s="3">
-        <v>0.32461852000000002</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B81" s="3">
-        <v>-0.18242923999999999</v>
+        <v>0.32461852000000002</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B82" s="3">
-        <v>0.31670985000000001</v>
+        <v>-0.18242923999999999</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B83" s="3">
-        <v>1.0607031200000001</v>
+        <v>0.31670985000000001</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B84" s="3">
-        <v>1.01682688</v>
+        <v>1.0607031200000001</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B85" s="3">
-        <v>1.28831315</v>
+        <v>1.01682688</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B86" s="3">
-        <v>0.18742834</v>
+        <v>1.28831315</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B87" s="3">
-        <v>0.51462112999999998</v>
+        <v>0.18742834</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B88" s="3">
-        <v>0.59033018000000004</v>
+        <v>0.51462112999999998</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B89" s="3">
-        <v>-0.98572367999999999</v>
+        <v>0.59033018000000004</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B90" s="3">
-        <v>-1.1165782099999999</v>
+        <v>-0.98572367999999999</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B91" s="3">
-        <v>-1.34219227</v>
+        <v>-1.1165782099999999</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B92" s="3">
-        <v>-1.8655826200000001</v>
+        <v>-1.34219227</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B93" s="3">
-        <v>-0.67636404999999999</v>
+        <v>-1.8655826200000001</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B94" s="3">
-        <v>0.42758853000000002</v>
+        <v>-0.67636404999999999</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B95" s="3">
-        <v>0.38266851000000002</v>
+        <v>0.42758853000000002</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B96" s="3">
-        <v>0.70743548000000001</v>
+        <v>0.38266851000000002</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.70743548000000001</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1669B248-4915-4C4D-A4FC-78BF0DEC8384}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add all debugging code and modifications
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Documents/code/aspire/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA27E7F-E37D-4E4B-83D8-F1602309590F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786C2E4C-AF5D-0445-BD48-1E945DF8853C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="196">
   <si>
     <t>name</t>
   </si>
@@ -597,9 +597,6 @@
     <t>Scale parameter term used in inverse logistic-like function to assign relative probability of having an HIV-positive male partner given age</t>
   </si>
   <si>
-    <t>Boily, 2009</t>
-  </si>
-  <si>
     <t>Calibrated in ABC model-fitting procedure with beta distribution with parameters alpha = 5 and beta = 1664, corresponding to point estimate and confidence interval reported for male-female-transmission in LMIC in Boily meta-analysis.</t>
   </si>
   <si>
@@ -610,6 +607,12 @@
   </si>
   <si>
     <t>rr_ring_partial_adh</t>
+  </si>
+  <si>
+    <t>Prior distribution bounds derived from Boily, 2009</t>
+  </si>
+  <si>
+    <t>Prior distribution bounds derived from Boily, 2009; Powers, 2008; Baggaley, 2010; and Patel, 2014</t>
   </si>
 </sst>
 </file>
@@ -981,7 +984,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,13 +1017,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>2.3224449999999998E-3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -1029,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>1.8</v>
+        <v>1.1416649999999999</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>185</v>
@@ -1044,7 +1047,7 @@
         <v>171</v>
       </c>
       <c r="B4" s="3">
-        <v>0.95</v>
+        <v>0.103786</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>172</v>
@@ -1059,7 +1062,7 @@
         <v>170</v>
       </c>
       <c r="B5" s="3">
-        <v>0.45</v>
+        <v>9.6844379999999994E-2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>172</v>
@@ -1074,12 +1077,14 @@
         <v>178</v>
       </c>
       <c r="B6" s="3">
-        <v>10</v>
+        <v>6.3494809999999999</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1110,26 +1115,26 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" s="3">
         <v>0.25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="3">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>

</xml_diff>

<commit_message>
Modifications for age- and time-specific incidence calibration
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Documents/code/aspire/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975F664A-D894-2549-8070-A6F8ADFCEB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B334EA-D979-F543-9B46-8CDA92EBEC9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -171,6 +172,36 @@
   </si>
   <si>
     <t>Prior distribution bounds derived from Boily, 2009; Powers, 2008; Baggaley, 2010; and Patel, 2014</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>mal_inc_ratio</t>
+  </si>
+  <si>
+    <t>uga_inc_ratio</t>
+  </si>
+  <si>
+    <t>zim_inc_ratio</t>
+  </si>
+  <si>
+    <t>rr_acute</t>
+  </si>
+  <si>
+    <t>Bellan, 2015</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with priors in uniform[1,20]</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with priors in uniform[0.0097,0.0988]</t>
+  </si>
+  <si>
+    <t>p_rate_rr</t>
+  </si>
+  <si>
+    <t>base_male_hiv_incidence</t>
   </si>
 </sst>
 </file>
@@ -241,12 +272,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>2.3224449999999998E-3</v>
+        <v>1.8884389552810601E-3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>41</v>
@@ -579,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>1.1416649999999999</v>
+        <v>1.13344954119313</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -594,7 +626,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2">
-        <v>0.103786</v>
+        <v>0.166659593977634</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>28</v>
@@ -609,7 +641,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="2">
-        <v>9.6844379999999994E-2</v>
+        <v>0.149284762235603</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -624,7 +656,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="2">
-        <v>6.3494809999999999</v>
+        <v>6.60051824979855</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>38</v>
@@ -636,88 +668,88 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2">
-        <v>2.89</v>
+        <v>5.4141890000000004</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2">
-        <v>0.96</v>
+        <v>8.5297999999999999E-2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
-        <v>0.25</v>
+        <v>2.89</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
-        <v>0.65</v>
+        <v>0.96</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2">
-        <v>2.5</v>
+        <v>0.65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2">
-        <v>3.63</v>
+        <v>0.22</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>35</v>
@@ -726,123 +758,203 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-1.4727514500000001</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1">
-        <v>-2.2884722900000001</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3.63</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.62259118000000002</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.75163418000000004</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2">
+        <f>0.22/1.21</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1">
-        <v>-0.28502549999999999</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2">
+        <f>0.31/1.21</f>
+        <v>0.256198347107438</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>-0.32447941000000002</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2">
+        <f>0.28/1.21</f>
+        <v>0.23140495867768598</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1">
-        <v>3.1312599999999999E-3</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>-1.4727514500000001</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
-        <v>1.5448442099999999</v>
+        <v>-2.2884722900000001</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.62259118000000002</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.75163418000000004</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-0.28502549999999999</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-0.32447941000000002</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.1312599999999999E-3</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.5448442099999999</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits for final simulations
</commit_message>
<xml_diff>
--- a/parameters/parameters.xlsx
+++ b/parameters/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpeebles/Documents/code/aspire/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9E1719-0CE7-4E4F-9F6E-3559BCC43419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFBC0F7-4E4B-CA40-B17C-E3AB57427CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28500" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -159,15 +159,9 @@
     <t>Calibrated in ABC model-fitting procedure with beta distribution with parameters alpha = 5 and beta = 1664, corresponding to point estimate and confidence interval reported for male-female-transmission in LMIC in Boily meta-analysis.</t>
   </si>
   <si>
-    <t>Brown, unpublished</t>
-  </si>
-  <si>
     <t>rr_ring_full_adh</t>
   </si>
   <si>
-    <t>rr_ring_partial_adh</t>
-  </si>
-  <si>
     <t>Prior distribution bounds derived from Boily, 2009</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>Bellan, 2015</t>
   </si>
   <si>
-    <t>Calibrated in ABC model-fitting procedure with priors in uniform[1,20]</t>
-  </si>
-  <si>
     <t>Calibrated in ABC model-fitting procedure with priors in uniform[0.0097,0.0988]</t>
   </si>
   <si>
@@ -199,12 +190,21 @@
   </si>
   <si>
     <t>base_male_hiv_incidence</t>
+  </si>
+  <si>
+    <t>Calibrated in ABC model-fitting procedure with priors in uniform[1,10]</t>
+  </si>
+  <si>
+    <t>Varied in simulations (default value here is always overridden)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -269,12 +269,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,11 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,14 +593,14 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.8884389552810601E-3</v>
+      <c r="B2" s="5">
+        <v>1.9868214403663902E-3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -606,8 +608,8 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.13344954119313</v>
+      <c r="B3" s="5">
+        <v>1.25499406094208</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -621,8 +623,8 @@
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.166659593977634</v>
+      <c r="B4" s="5">
+        <v>0.16839003020767901</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>28</v>
@@ -636,8 +638,8 @@
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.149284762235603</v>
+      <c r="B5" s="5">
+        <v>0.15167522244342599</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -651,39 +653,39 @@
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="2">
-        <v>6.60051824979855</v>
+      <c r="B6" s="5">
+        <v>6.9262904468113398</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5.4141890000000004</v>
+        <v>51</v>
+      </c>
+      <c r="B7" s="5">
+        <v>8.0637087324821195</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2">
-        <v>8.5297999999999999E-2</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8.7470956280958606E-2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -716,36 +718,36 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2">
         <v>0.25</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2">
-        <v>0.65</v>
+        <v>0.22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2">
-        <v>0.22</v>
+        <v>2.5</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>35</v>
@@ -755,10 +757,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
-        <v>2.5</v>
+        <v>3.63</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
@@ -768,37 +770,36 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2">
-        <v>3.63</v>
+        <v>5.3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2">
-        <v>5.3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B16" s="5">
+        <f>0.22/1.21</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="2">
-        <f>0.22/1.21</f>
-        <v>0.18181818181818182</v>
+        <v>46</v>
+      </c>
+      <c r="B17" s="5">
+        <f>0.31/1.21</f>
+        <v>0.256198347107438</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -806,53 +807,56 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="2">
-        <f>0.31/1.21</f>
-        <v>0.256198347107438</v>
+        <v>47</v>
+      </c>
+      <c r="B18" s="5">
+        <f>0.28/1.21</f>
+        <v>0.23140495867768598</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="2">
-        <f>0.28/1.21</f>
-        <v>0.23140495867768598</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-1.4727514500000001</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>-1.4727514500000001</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-2.2884722900000001</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1">
-        <v>-2.2884722900000001</v>
+        <v>8</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.62259118000000002</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>25</v>
@@ -860,14 +864,14 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.62259118000000002</v>
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.75163418000000004</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>25</v>
@@ -875,29 +879,29 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.75163418000000004</v>
+        <v>10</v>
+      </c>
+      <c r="B23" s="6">
+        <v>-0.28502549999999999</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="1">
-        <v>-0.28502549999999999</v>
+        <v>11</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-0.32447941000000002</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>24</v>
@@ -905,14 +909,14 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="1">
-        <v>-0.32447941000000002</v>
+        <v>12</v>
+      </c>
+      <c r="B25" s="6">
+        <v>3.1312599999999999E-3</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
@@ -920,31 +924,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3.1312599999999999E-3</v>
+        <v>13</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1.5448442099999999</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.5448442099999999</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>